<commit_message>
Batch update 2025-10-29 13:54
</commit_message>
<xml_diff>
--- a/flagged_segments.xlsx
+++ b/flagged_segments.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="74">
   <si>
     <t>Session</t>
   </si>
@@ -34,22 +34,205 @@
     <t>GMT20250821-130122</t>
   </si>
   <si>
+    <t>No, you don't know, because you haven't started reading it yet.</t>
+  </si>
+  <si>
+    <t>Later on, under… Do you remember what that was called?</t>
+  </si>
+  <si>
+    <t>I think they lost the war.</t>
+  </si>
+  <si>
+    <t>Yeah, but that's what I'm saying, though. That's making the connection, though. Why? Why Portugal?</t>
+  </si>
+  <si>
+    <t>And later, tobacco.</t>
+  </si>
+  <si>
+    <t>And later, cotton.</t>
+  </si>
+  <si>
+    <t>Yeah, that becomes important a little bit later, because the Japanese invade Manchuria, And they call it Manchuko.</t>
+  </si>
+  <si>
     <t>Yeah, because they were guaranteed, like, a future.</t>
   </si>
   <si>
     <t>I think the Magna Carta, guarantees rights to Like,</t>
   </si>
   <si>
+    <t>No worries, because I do not judge you, and I don't know what your lifestyle is like, or how busy you were, or what your weekend was, but what my job is to make sure that you see this from a bigger perspective, and realize that it's not complicated.</t>
+  </si>
+  <si>
+    <t>Yes, I am giving you the bigger picture idea. And I say Unit 4, pay attention to Unit 4, because the Columbian Exchange</t>
+  </si>
+  <si>
+    <t>Hi, can you hear me?</t>
+  </si>
+  <si>
+    <t>… can't… oh, can you hear me?</t>
+  </si>
+  <si>
+    <t>Hello, can you hear me? I can hear you.</t>
+  </si>
+  <si>
+    <t>Yes, can you hear me?</t>
+  </si>
+  <si>
+    <t>Can you hear me?</t>
+  </si>
+  <si>
+    <t>I can, yeah, but can you hear me?</t>
+  </si>
+  <si>
+    <t>Oh, interesting. I'll double-check my audio, but I think… oh, you can't hear me, one second.</t>
+  </si>
+  <si>
+    <t>Hello? I don't know if you can hear me, but I'll leave the call and just join back.</t>
+  </si>
+  <si>
+    <t>Oh, alright, awesome. Yes, I can hear you, can you hear me?</t>
+  </si>
+  <si>
+    <t>Oh, I see, I see, okay. Good. But is it lagging? Is the Wi-Fi fine now?</t>
+  </si>
+  <si>
+    <t>Okay, can you hear me properly, by the way?</t>
+  </si>
+  <si>
+    <t>And we focused mainly on altering conditions, altering, what's it called, concentrations. There are other conditions that we can alter when it comes to equilibria, including pressure, and that has to do with gases, right? Because gases</t>
+  </si>
+  <si>
+    <t>I'm not sure. I….</t>
+  </si>
+  <si>
+    <t>Can you hear me properly? I can't tell if I'm lagging or not.</t>
+  </si>
+  <si>
+    <t>I am definitely lagging. Or, or I don't know, there's something off.</t>
+  </si>
+  <si>
+    <t>Hello, can you hear me?</t>
+  </si>
+  <si>
+    <t>Yeah, can you hear me better now?</t>
+  </si>
+  <si>
+    <t>Okay, if at some point it starts lagging to the point where you're not understanding what I'm saying.</t>
+  </si>
+  <si>
+    <t>find another meeting room. I don't know.</t>
+  </si>
+  <si>
+    <t>Hello? Oh my god, I'm… I don't know what's happening. …</t>
+  </si>
+  <si>
+    <t>Yeah, I can't tell… I can't tell if I'm the one that's lagging, or if it's your… if it's your Wi-Fi, I'm….</t>
+  </si>
+  <si>
+    <t>Instead of having this happen all… I don't know.</t>
+  </si>
+  <si>
+    <t>Yes, yes, yes, I can… can you hear me still?</t>
+  </si>
+  <si>
+    <t>Yes, can you hear me still?</t>
+  </si>
+  <si>
+    <t>Okay, can you hear me now?</t>
+  </si>
+  <si>
+    <t>Oh my god, I'm so sorry, I don't know why. Some meeting rooms… in some meeting rooms in my department, the connection is weird. If I start lagging at any point, let me know again. But yeah, we lost, like.</t>
+  </si>
+  <si>
+    <t>I think I'm still lagging. Oh my god.</t>
+  </si>
+  <si>
+    <t>I think I'm still lagging, am I not?</t>
+  </si>
+  <si>
+    <t>It's unfair to you if we just go on like this for the next 30, 40 minutes of this session. If the internet issue continues happening, then I'll just ask them to, like, not charge you for the session. Hello? Can you hear me?</t>
+  </si>
+  <si>
+    <t>Yeah, yeah. Can you hear me?</t>
+  </si>
+  <si>
+    <t>Yeah, I don't know what to do. So I'll just… ask…</t>
+  </si>
+  <si>
+    <t>So, would you… I think it's unfair to you… let's try to go on for 5 minutes. Can you hear me… can you hear what I'm saying?</t>
+  </si>
+  <si>
+    <t>And I'm not sure it will get resolved in the next 30 minutes.</t>
+  </si>
+  <si>
+    <t>Is that fine? I think it's just unfair to you that I just talk and you spend, like, half the time deciphering what I'm saying because of internet issues.</t>
+  </si>
+  <si>
     <t>having, you know, like, the next 30 minutes, and also not being 100% sure, you'll hear what I'm saying in the next 30 minutes.</t>
   </si>
   <si>
+    <t>Can you hear me properly?</t>
+  </si>
+  <si>
+    <t>Can you hear me, by the way? I know I've asked, like, a million times, but I… You're good.</t>
+  </si>
+  <si>
+    <t>By the way, I just want to put the option forward. Would you rather that we… like… just…</t>
+  </si>
+  <si>
+    <t>Yeah, I can see stuff, but I think maybe… I don't know if it's writing properly, or if it's….</t>
+  </si>
+  <si>
+    <t>I can't hear… I can't hear anything. God, I… yeah, I don't know how this is gonna work.</t>
+  </si>
+  <si>
+    <t>Yes, I can hear you. Can you hear me?</t>
+  </si>
+  <si>
+    <t>I am writing. Maybe it'll appear for you on a… in a bit, I'm not sure.</t>
+  </si>
+  <si>
+    <t>Yeah, can you hear me again? Oh my god. I honestly think this is completely horrible for you, like, I feel so bad. I think this is just not… I think this is gonna be the case for the next, like, 15 minutes or so. …</t>
+  </si>
+  <si>
+    <t>It's not the best use of your time as well. I feel so bad, I'm so sorry. I don't know what happened to this wife situation. So, I'll make sure they don't charge you for it, because we literally covered, like.</t>
+  </si>
+  <si>
+    <t>Yes, yes, yeah, I'm just apologizing again, and please also apologize to your parents for me, but we'll make sure to sort this out with the team, and we'll do a makeup class for sure.</t>
+  </si>
+  <si>
     <t>https://andreamaria810.github.io/Zoom_Reports/html_reports/GMT20251026-075624_report.html</t>
   </si>
   <si>
     <t>https://andreamaria810.github.io/Zoom_Reports/html_reports/GMT20250821-130122_report.html</t>
   </si>
   <si>
-    <t>risk</t>
+    <t>Session Quality: Tutor Knowledge Gaps</t>
+  </si>
+  <si>
+    <t>Student Behavior Issues: Student Late</t>
+  </si>
+  <si>
+    <t>Session Quality: Not Understanding Material</t>
+  </si>
+  <si>
+    <t>Technical: Connectivity Issues</t>
+  </si>
+  <si>
+    <t>Tutor Policy Breach: Over-Promising</t>
+  </si>
+  <si>
+    <t>Session Quality: Lack of Engagement</t>
+  </si>
+  <si>
+    <t>Technical: Audio Issues</t>
+  </si>
+  <si>
+    <t>Session Quality: Off-Topic Discussion</t>
+  </si>
+  <si>
+    <t>Other: Parent Over-Involvement</t>
   </si>
   <si>
     <t>View Report</t>
@@ -419,7 +602,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -453,10 +636,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -467,24 +650,836 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
+      <c r="C8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D48" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D51" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D52" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D53" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D54" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D55" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" t="s">
+        <v>57</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D57" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" t="s">
+        <v>58</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D58" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" t="s">
+        <v>59</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" t="s">
+        <v>60</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D60" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" t="s">
+        <v>32</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D61" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" t="s">
+        <v>61</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D62" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -492,6 +1487,64 @@
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C12" r:id="rId11"/>
+    <hyperlink ref="C13" r:id="rId12"/>
+    <hyperlink ref="C14" r:id="rId13"/>
+    <hyperlink ref="C15" r:id="rId14"/>
+    <hyperlink ref="C16" r:id="rId15"/>
+    <hyperlink ref="C17" r:id="rId16"/>
+    <hyperlink ref="C18" r:id="rId17"/>
+    <hyperlink ref="C19" r:id="rId18"/>
+    <hyperlink ref="C20" r:id="rId19"/>
+    <hyperlink ref="C21" r:id="rId20"/>
+    <hyperlink ref="C22" r:id="rId21"/>
+    <hyperlink ref="C23" r:id="rId22"/>
+    <hyperlink ref="C24" r:id="rId23"/>
+    <hyperlink ref="C25" r:id="rId24"/>
+    <hyperlink ref="C26" r:id="rId25"/>
+    <hyperlink ref="C27" r:id="rId26"/>
+    <hyperlink ref="C28" r:id="rId27"/>
+    <hyperlink ref="C29" r:id="rId28"/>
+    <hyperlink ref="C30" r:id="rId29"/>
+    <hyperlink ref="C31" r:id="rId30"/>
+    <hyperlink ref="C32" r:id="rId31"/>
+    <hyperlink ref="C33" r:id="rId32"/>
+    <hyperlink ref="C34" r:id="rId33"/>
+    <hyperlink ref="C35" r:id="rId34"/>
+    <hyperlink ref="C36" r:id="rId35"/>
+    <hyperlink ref="C37" r:id="rId36"/>
+    <hyperlink ref="C38" r:id="rId37"/>
+    <hyperlink ref="C39" r:id="rId38"/>
+    <hyperlink ref="C40" r:id="rId39"/>
+    <hyperlink ref="C41" r:id="rId40"/>
+    <hyperlink ref="C42" r:id="rId41"/>
+    <hyperlink ref="C43" r:id="rId42"/>
+    <hyperlink ref="C44" r:id="rId43"/>
+    <hyperlink ref="C45" r:id="rId44"/>
+    <hyperlink ref="C46" r:id="rId45"/>
+    <hyperlink ref="C47" r:id="rId46"/>
+    <hyperlink ref="C48" r:id="rId47"/>
+    <hyperlink ref="C49" r:id="rId48"/>
+    <hyperlink ref="C50" r:id="rId49"/>
+    <hyperlink ref="C51" r:id="rId50"/>
+    <hyperlink ref="C52" r:id="rId51"/>
+    <hyperlink ref="C53" r:id="rId52"/>
+    <hyperlink ref="C54" r:id="rId53"/>
+    <hyperlink ref="C55" r:id="rId54"/>
+    <hyperlink ref="C56" r:id="rId55"/>
+    <hyperlink ref="C57" r:id="rId56"/>
+    <hyperlink ref="C58" r:id="rId57"/>
+    <hyperlink ref="C59" r:id="rId58"/>
+    <hyperlink ref="C60" r:id="rId59"/>
+    <hyperlink ref="C61" r:id="rId60"/>
+    <hyperlink ref="C62" r:id="rId61"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Validated report update 2025-10-29 17:51
</commit_message>
<xml_diff>
--- a/flagged_segments.xlsx
+++ b/flagged_segments.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="60">
   <si>
     <t>Session</t>
   </si>
@@ -37,30 +37,12 @@
     <t>No, you don't know, because you haven't started reading it yet.</t>
   </si>
   <si>
-    <t>Later on, under… Do you remember what that was called?</t>
-  </si>
-  <si>
     <t>I think they lost the war.</t>
   </si>
   <si>
-    <t>Yeah, but that's what I'm saying, though. That's making the connection, though. Why? Why Portugal?</t>
-  </si>
-  <si>
-    <t>And later, tobacco.</t>
-  </si>
-  <si>
-    <t>And later, cotton.</t>
-  </si>
-  <si>
-    <t>Yeah, that becomes important a little bit later, because the Japanese invade Manchuria, And they call it Manchuko.</t>
-  </si>
-  <si>
     <t>Yeah, because they were guaranteed, like, a future.</t>
   </si>
   <si>
-    <t>I think the Magna Carta, guarantees rights to Like,</t>
-  </si>
-  <si>
     <t>No worries, because I do not judge you, and I don't know what your lifestyle is like, or how busy you were, or what your weekend was, but what my job is to make sure that you see this from a bigger perspective, and realize that it's not complicated.</t>
   </si>
   <si>
@@ -88,18 +70,12 @@
     <t>Oh, interesting. I'll double-check my audio, but I think… oh, you can't hear me, one second.</t>
   </si>
   <si>
-    <t>Hello? I don't know if you can hear me, but I'll leave the call and just join back.</t>
-  </si>
-  <si>
     <t>Oh, alright, awesome. Yes, I can hear you, can you hear me?</t>
   </si>
   <si>
     <t>Oh, I see, I see, okay. Good. But is it lagging? Is the Wi-Fi fine now?</t>
   </si>
   <si>
-    <t>Okay, can you hear me properly, by the way?</t>
-  </si>
-  <si>
     <t>And we focused mainly on altering conditions, altering, what's it called, concentrations. There are other conditions that we can alter when it comes to equilibria, including pressure, and that has to do with gases, right? Because gases</t>
   </si>
   <si>
@@ -112,30 +88,21 @@
     <t>I am definitely lagging. Or, or I don't know, there's something off.</t>
   </si>
   <si>
+    <t>Yeah, can you hear me better now?</t>
+  </si>
+  <si>
+    <t>Okay, if at some point it starts lagging to the point where you're not understanding what I'm saying.</t>
+  </si>
+  <si>
+    <t>find another meeting room. I don't know.</t>
+  </si>
+  <si>
     <t>Hello, can you hear me?</t>
   </si>
   <si>
-    <t>Yeah, can you hear me better now?</t>
-  </si>
-  <si>
-    <t>Okay, if at some point it starts lagging to the point where you're not understanding what I'm saying.</t>
-  </si>
-  <si>
-    <t>find another meeting room. I don't know.</t>
-  </si>
-  <si>
-    <t>Hello? Oh my god, I'm… I don't know what's happening. …</t>
-  </si>
-  <si>
     <t>Yeah, I can't tell… I can't tell if I'm the one that's lagging, or if it's your… if it's your Wi-Fi, I'm….</t>
   </si>
   <si>
-    <t>Instead of having this happen all… I don't know.</t>
-  </si>
-  <si>
-    <t>Yes, yes, yes, I can… can you hear me still?</t>
-  </si>
-  <si>
     <t>Yes, can you hear me still?</t>
   </si>
   <si>
@@ -187,12 +154,6 @@
     <t>I can't hear… I can't hear anything. God, I… yeah, I don't know how this is gonna work.</t>
   </si>
   <si>
-    <t>Yes, I can hear you. Can you hear me?</t>
-  </si>
-  <si>
-    <t>I am writing. Maybe it'll appear for you on a… in a bit, I'm not sure.</t>
-  </si>
-  <si>
     <t>Yeah, can you hear me again? Oh my god. I honestly think this is completely horrible for you, like, I feel so bad. I think this is just not… I think this is gonna be the case for the next, like, 15 minutes or so. …</t>
   </si>
   <si>
@@ -202,31 +163,28 @@
     <t>Yes, yes, yeah, I'm just apologizing again, and please also apologize to your parents for me, but we'll make sure to sort this out with the team, and we'll do a makeup class for sure.</t>
   </si>
   <si>
-    <t>https://andreamaria810.github.io/Zoom_Reports/html_reports/GMT20251026-075624_report.html</t>
-  </si>
-  <si>
-    <t>https://andreamaria810.github.io/Zoom_Reports/html_reports/GMT20250821-130122_report.html</t>
+    <t>https://andreamaria810.github.io/Zoom_Reports/html_reports/GMT20251026-075624_validated_report.html</t>
+  </si>
+  <si>
+    <t>https://andreamaria810.github.io/Zoom_Reports/html_reports/GMT20250821-130122_validated_report.html</t>
   </si>
   <si>
     <t>Session Quality: Tutor Knowledge Gaps</t>
   </si>
   <si>
-    <t>Student Behavior Issues: Student Late</t>
-  </si>
-  <si>
     <t>Session Quality: Not Understanding Material</t>
   </si>
   <si>
+    <t>Tutor Policy Breach: Over-Promising</t>
+  </si>
+  <si>
+    <t>Session Quality: Lack of Engagement</t>
+  </si>
+  <si>
+    <t>Technical: Audio Issues</t>
+  </si>
+  <si>
     <t>Technical: Connectivity Issues</t>
-  </si>
-  <si>
-    <t>Tutor Policy Breach: Over-Promising</t>
-  </si>
-  <si>
-    <t>Session Quality: Lack of Engagement</t>
-  </si>
-  <si>
-    <t>Technical: Audio Issues</t>
   </si>
   <si>
     <t>Session Quality: Off-Topic Discussion</t>
@@ -602,7 +560,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -636,10 +594,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -650,10 +608,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -664,10 +622,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -678,10 +636,10 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -692,94 +650,94 @@
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -790,10 +748,10 @@
         <v>17</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -801,13 +759,13 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -815,13 +773,13 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -829,13 +787,13 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -843,13 +801,13 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -857,13 +815,13 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -871,13 +829,13 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D19" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -885,13 +843,13 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -899,13 +857,13 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -916,10 +874,10 @@
         <v>25</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -930,10 +888,10 @@
         <v>26</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -944,10 +902,10 @@
         <v>27</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D24" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -958,10 +916,10 @@
         <v>28</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -972,10 +930,10 @@
         <v>29</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D26" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -986,10 +944,10 @@
         <v>30</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D27" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1000,10 +958,10 @@
         <v>31</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D28" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1014,10 +972,10 @@
         <v>32</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D29" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1028,10 +986,10 @@
         <v>33</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D30" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1042,10 +1000,10 @@
         <v>34</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D31" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1056,10 +1014,10 @@
         <v>35</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D32" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1070,10 +1028,10 @@
         <v>36</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D33" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1081,13 +1039,13 @@
         <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D34" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1095,13 +1053,13 @@
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D35" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1109,13 +1067,13 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D36" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1123,13 +1081,13 @@
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D37" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1137,13 +1095,13 @@
         <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D38" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1151,13 +1109,13 @@
         <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D39" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1165,13 +1123,13 @@
         <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D40" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1179,13 +1137,13 @@
         <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D41" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1193,13 +1151,13 @@
         <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D42" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1207,13 +1165,13 @@
         <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D43" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1221,13 +1179,13 @@
         <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D44" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1235,13 +1193,13 @@
         <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D45" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1249,13 +1207,13 @@
         <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D46" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1263,223 +1221,13 @@
         <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D47" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" t="s">
-        <v>5</v>
-      </c>
-      <c r="B48" t="s">
-        <v>50</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D48" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" t="s">
-        <v>5</v>
-      </c>
-      <c r="B49" t="s">
-        <v>51</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D49" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" t="s">
-        <v>5</v>
-      </c>
-      <c r="B50" t="s">
-        <v>52</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D50" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" t="s">
-        <v>5</v>
-      </c>
-      <c r="B51" t="s">
-        <v>53</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D51" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52" t="s">
-        <v>54</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D52" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" t="s">
-        <v>5</v>
-      </c>
-      <c r="B53" t="s">
-        <v>55</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D53" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" t="s">
-        <v>5</v>
-      </c>
-      <c r="B54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D54" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" t="s">
-        <v>5</v>
-      </c>
-      <c r="B55" t="s">
-        <v>21</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D55" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
-        <v>5</v>
-      </c>
-      <c r="B56" t="s">
-        <v>56</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D56" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" t="s">
-        <v>5</v>
-      </c>
-      <c r="B57" t="s">
-        <v>57</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D57" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" t="s">
-        <v>5</v>
-      </c>
-      <c r="B58" t="s">
         <v>58</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" t="s">
-        <v>5</v>
-      </c>
-      <c r="B59" t="s">
-        <v>59</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D59" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" t="s">
-        <v>5</v>
-      </c>
-      <c r="B60" t="s">
-        <v>60</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D60" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" t="s">
-        <v>5</v>
-      </c>
-      <c r="B61" t="s">
-        <v>32</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D61" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" t="s">
-        <v>5</v>
-      </c>
-      <c r="B62" t="s">
-        <v>61</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D62" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1530,21 +1278,6 @@
     <hyperlink ref="C45" r:id="rId44"/>
     <hyperlink ref="C46" r:id="rId45"/>
     <hyperlink ref="C47" r:id="rId46"/>
-    <hyperlink ref="C48" r:id="rId47"/>
-    <hyperlink ref="C49" r:id="rId48"/>
-    <hyperlink ref="C50" r:id="rId49"/>
-    <hyperlink ref="C51" r:id="rId50"/>
-    <hyperlink ref="C52" r:id="rId51"/>
-    <hyperlink ref="C53" r:id="rId52"/>
-    <hyperlink ref="C54" r:id="rId53"/>
-    <hyperlink ref="C55" r:id="rId54"/>
-    <hyperlink ref="C56" r:id="rId55"/>
-    <hyperlink ref="C57" r:id="rId56"/>
-    <hyperlink ref="C58" r:id="rId57"/>
-    <hyperlink ref="C59" r:id="rId58"/>
-    <hyperlink ref="C60" r:id="rId59"/>
-    <hyperlink ref="C61" r:id="rId60"/>
-    <hyperlink ref="C62" r:id="rId61"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Validated report update 2025-10-29 20:44
</commit_message>
<xml_diff>
--- a/flagged_segments.xlsx
+++ b/flagged_segments.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="57">
   <si>
     <t>Session</t>
   </si>
@@ -55,9 +55,6 @@
     <t>… can't… oh, can you hear me?</t>
   </si>
   <si>
-    <t>Hello, can you hear me? I can hear you.</t>
-  </si>
-  <si>
     <t>Yes, can you hear me?</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
     <t>Oh, interesting. I'll double-check my audio, but I think… oh, you can't hear me, one second.</t>
   </si>
   <si>
+    <t>Hello? I don't know if you can hear me, but I'll leave the call and just join back.</t>
+  </si>
+  <si>
     <t>Oh, alright, awesome. Yes, I can hear you, can you hear me?</t>
   </si>
   <si>
@@ -94,9 +94,6 @@
     <t>Okay, if at some point it starts lagging to the point where you're not understanding what I'm saying.</t>
   </si>
   <si>
-    <t>find another meeting room. I don't know.</t>
-  </si>
-  <si>
     <t>Hello, can you hear me?</t>
   </si>
   <si>
@@ -112,9 +109,6 @@
     <t>Oh my god, I'm so sorry, I don't know why. Some meeting rooms… in some meeting rooms in my department, the connection is weird. If I start lagging at any point, let me know again. But yeah, we lost, like.</t>
   </si>
   <si>
-    <t>I think I'm still lagging. Oh my god.</t>
-  </si>
-  <si>
     <t>I think I'm still lagging, am I not?</t>
   </si>
   <si>
@@ -133,18 +127,12 @@
     <t>And I'm not sure it will get resolved in the next 30 minutes.</t>
   </si>
   <si>
-    <t>Is that fine? I think it's just unfair to you that I just talk and you spend, like, half the time deciphering what I'm saying because of internet issues.</t>
-  </si>
-  <si>
     <t>having, you know, like, the next 30 minutes, and also not being 100% sure, you'll hear what I'm saying in the next 30 minutes.</t>
   </si>
   <si>
     <t>Can you hear me properly?</t>
   </si>
   <si>
-    <t>Can you hear me, by the way? I know I've asked, like, a million times, but I… You're good.</t>
-  </si>
-  <si>
     <t>By the way, I just want to put the option forward. Would you rather that we… like… just…</t>
   </si>
   <si>
@@ -152,6 +140,9 @@
   </si>
   <si>
     <t>I can't hear… I can't hear anything. God, I… yeah, I don't know how this is gonna work.</t>
+  </si>
+  <si>
+    <t>Yes, I can hear you. Can you hear me?</t>
   </si>
   <si>
     <t>Yeah, can you hear me again? Oh my god. I honestly think this is completely horrible for you, like, I feel so bad. I think this is just not… I think this is gonna be the case for the next, like, 15 minutes or so. …</t>
@@ -560,7 +551,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -594,10 +585,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -608,10 +599,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -622,10 +613,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -636,10 +627,10 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -650,10 +641,10 @@
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -664,10 +655,10 @@
         <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -678,10 +669,10 @@
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -692,10 +683,10 @@
         <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -706,10 +697,10 @@
         <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -720,10 +711,10 @@
         <v>15</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -734,10 +725,10 @@
         <v>16</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -748,10 +739,10 @@
         <v>17</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -759,13 +750,13 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -776,10 +767,10 @@
         <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -790,10 +781,10 @@
         <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -804,10 +795,10 @@
         <v>20</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -818,10 +809,10 @@
         <v>21</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -832,10 +823,10 @@
         <v>22</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -846,10 +837,10 @@
         <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -860,10 +851,10 @@
         <v>24</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -874,10 +865,10 @@
         <v>25</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -888,10 +879,10 @@
         <v>26</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -902,10 +893,10 @@
         <v>27</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -916,10 +907,10 @@
         <v>28</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -930,10 +921,10 @@
         <v>29</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -944,10 +935,10 @@
         <v>30</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -958,10 +949,10 @@
         <v>31</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D28" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -972,10 +963,10 @@
         <v>32</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D29" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -986,10 +977,10 @@
         <v>33</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D30" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1000,10 +991,10 @@
         <v>34</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1014,10 +1005,10 @@
         <v>35</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1028,10 +1019,10 @@
         <v>36</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D33" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1042,10 +1033,10 @@
         <v>37</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D34" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1056,10 +1047,10 @@
         <v>38</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D35" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1070,10 +1061,10 @@
         <v>39</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D36" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1084,10 +1075,10 @@
         <v>40</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D37" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1095,13 +1086,13 @@
         <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D38" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1109,13 +1100,13 @@
         <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D39" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1123,13 +1114,13 @@
         <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D40" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1137,13 +1128,13 @@
         <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D41" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1151,13 +1142,13 @@
         <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D42" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1165,13 +1156,13 @@
         <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D43" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1179,13 +1170,13 @@
         <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D44" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1193,41 +1184,13 @@
         <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D45" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" t="s">
-        <v>5</v>
-      </c>
-      <c r="B46" t="s">
-        <v>47</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D46" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" t="s">
-        <v>5</v>
-      </c>
-      <c r="B47" t="s">
-        <v>48</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D47" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1276,8 +1239,6 @@
     <hyperlink ref="C43" r:id="rId42"/>
     <hyperlink ref="C44" r:id="rId43"/>
     <hyperlink ref="C45" r:id="rId44"/>
-    <hyperlink ref="C46" r:id="rId45"/>
-    <hyperlink ref="C47" r:id="rId46"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Validated report update 2025-10-29 23:35
</commit_message>
<xml_diff>
--- a/flagged_segments.xlsx
+++ b/flagged_segments.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="70">
   <si>
     <t>Session</t>
   </si>
@@ -37,12 +37,30 @@
     <t>No, you don't know, because you haven't started reading it yet.</t>
   </si>
   <si>
+    <t>Later on, under… Do you remember what that was called?</t>
+  </si>
+  <si>
     <t>I think they lost the war.</t>
   </si>
   <si>
+    <t>Yeah, but that's what I'm saying, though. That's making the connection, though. Why? Why Portugal?</t>
+  </si>
+  <si>
+    <t>And later, tobacco.</t>
+  </si>
+  <si>
+    <t>And later, cotton.</t>
+  </si>
+  <si>
+    <t>Yeah, that becomes important a little bit later, because the Japanese invade Manchuria, And they call it Manchuko.</t>
+  </si>
+  <si>
     <t>Yeah, because they were guaranteed, like, a future.</t>
   </si>
   <si>
+    <t>I think the Magna Carta, guarantees rights to Like,</t>
+  </si>
+  <si>
     <t>No worries, because I do not judge you, and I don't know what your lifestyle is like, or how busy you were, or what your weekend was, but what my job is to make sure that you see this from a bigger perspective, and realize that it's not complicated.</t>
   </si>
   <si>
@@ -55,6 +73,9 @@
     <t>… can't… oh, can you hear me?</t>
   </si>
   <si>
+    <t>Hello, can you hear me? I can hear you.</t>
+  </si>
+  <si>
     <t>Yes, can you hear me?</t>
   </si>
   <si>
@@ -76,6 +97,9 @@
     <t>Oh, I see, I see, okay. Good. But is it lagging? Is the Wi-Fi fine now?</t>
   </si>
   <si>
+    <t>Okay, can you hear me properly, by the way?</t>
+  </si>
+  <si>
     <t>And we focused mainly on altering conditions, altering, what's it called, concentrations. There are other conditions that we can alter when it comes to equilibria, including pressure, and that has to do with gases, right? Because gases</t>
   </si>
   <si>
@@ -88,18 +112,27 @@
     <t>I am definitely lagging. Or, or I don't know, there's something off.</t>
   </si>
   <si>
+    <t>Hello, can you hear me?</t>
+  </si>
+  <si>
     <t>Yeah, can you hear me better now?</t>
   </si>
   <si>
     <t>Okay, if at some point it starts lagging to the point where you're not understanding what I'm saying.</t>
   </si>
   <si>
-    <t>Hello, can you hear me?</t>
+    <t>Hello? Oh my god, I'm… I don't know what's happening. …</t>
   </si>
   <si>
     <t>Yeah, I can't tell… I can't tell if I'm the one that's lagging, or if it's your… if it's your Wi-Fi, I'm….</t>
   </si>
   <si>
+    <t>Instead of having this happen all… I don't know.</t>
+  </si>
+  <si>
+    <t>Yes, yes, yes, I can… can you hear me still?</t>
+  </si>
+  <si>
     <t>Yes, can you hear me still?</t>
   </si>
   <si>
@@ -109,30 +142,30 @@
     <t>Oh my god, I'm so sorry, I don't know why. Some meeting rooms… in some meeting rooms in my department, the connection is weird. If I start lagging at any point, let me know again. But yeah, we lost, like.</t>
   </si>
   <si>
+    <t>I think I'm still lagging. Oh my god.</t>
+  </si>
+  <si>
     <t>I think I'm still lagging, am I not?</t>
   </si>
   <si>
-    <t>It's unfair to you if we just go on like this for the next 30, 40 minutes of this session. If the internet issue continues happening, then I'll just ask them to, like, not charge you for the session. Hello? Can you hear me?</t>
-  </si>
-  <si>
     <t>Yeah, yeah. Can you hear me?</t>
   </si>
   <si>
-    <t>Yeah, I don't know what to do. So I'll just… ask…</t>
-  </si>
-  <si>
     <t>So, would you… I think it's unfair to you… let's try to go on for 5 minutes. Can you hear me… can you hear what I'm saying?</t>
   </si>
   <si>
     <t>And I'm not sure it will get resolved in the next 30 minutes.</t>
   </si>
   <si>
-    <t>having, you know, like, the next 30 minutes, and also not being 100% sure, you'll hear what I'm saying in the next 30 minutes.</t>
+    <t>Is that fine? I think it's just unfair to you that I just talk and you spend, like, half the time deciphering what I'm saying because of internet issues.</t>
   </si>
   <si>
     <t>Can you hear me properly?</t>
   </si>
   <si>
+    <t>Can you hear me, by the way? I know I've asked, like, a million times, but I… You're good.</t>
+  </si>
+  <si>
     <t>By the way, I just want to put the option forward. Would you rather that we… like… just…</t>
   </si>
   <si>
@@ -145,6 +178,9 @@
     <t>Yes, I can hear you. Can you hear me?</t>
   </si>
   <si>
+    <t>I am writing. Maybe it'll appear for you on a… in a bit, I'm not sure.</t>
+  </si>
+  <si>
     <t>Yeah, can you hear me again? Oh my god. I honestly think this is completely horrible for you, like, I feel so bad. I think this is just not… I think this is gonna be the case for the next, like, 15 minutes or so. …</t>
   </si>
   <si>
@@ -163,9 +199,15 @@
     <t>Session Quality: Tutor Knowledge Gaps</t>
   </si>
   <si>
+    <t>Student Behavior Issues: Student Late</t>
+  </si>
+  <si>
     <t>Session Quality: Not Understanding Material</t>
   </si>
   <si>
+    <t>Technical: Connectivity Issues</t>
+  </si>
+  <si>
     <t>Tutor Policy Breach: Over-Promising</t>
   </si>
   <si>
@@ -173,9 +215,6 @@
   </si>
   <si>
     <t>Technical: Audio Issues</t>
-  </si>
-  <si>
-    <t>Technical: Connectivity Issues</t>
   </si>
   <si>
     <t>Session Quality: Off-Topic Discussion</t>
@@ -551,7 +590,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -585,10 +624,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -599,10 +638,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -613,10 +652,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -627,10 +666,10 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -641,94 +680,94 @@
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -739,10 +778,10 @@
         <v>17</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -750,13 +789,13 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -764,13 +803,13 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -778,13 +817,13 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -792,13 +831,13 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -806,13 +845,13 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -820,13 +859,13 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -834,13 +873,13 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -848,13 +887,13 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D21" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -865,10 +904,10 @@
         <v>25</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -879,10 +918,10 @@
         <v>26</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -893,10 +932,10 @@
         <v>27</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -907,10 +946,10 @@
         <v>28</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -921,10 +960,10 @@
         <v>29</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D26" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -935,10 +974,10 @@
         <v>30</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D27" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -949,10 +988,10 @@
         <v>31</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D28" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -963,10 +1002,10 @@
         <v>32</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D29" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -977,10 +1016,10 @@
         <v>33</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D30" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -991,10 +1030,10 @@
         <v>34</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D31" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1005,10 +1044,10 @@
         <v>35</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D32" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1016,13 +1055,13 @@
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D33" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1030,13 +1069,13 @@
         <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D34" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1044,13 +1083,13 @@
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D35" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1058,13 +1097,13 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D36" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1072,13 +1111,13 @@
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D37" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1086,13 +1125,13 @@
         <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D38" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1100,13 +1139,13 @@
         <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D39" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1114,13 +1153,13 @@
         <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D40" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1128,13 +1167,13 @@
         <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D41" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1142,13 +1181,13 @@
         <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D42" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1156,13 +1195,13 @@
         <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D43" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1170,13 +1209,13 @@
         <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D44" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1184,13 +1223,195 @@
         <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C45" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D50" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D51" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D52" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" t="s">
+        <v>53</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D53" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" t="s">
+        <v>54</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D54" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D55" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" t="s">
         <v>56</v>
       </c>
-      <c r="D45" t="s">
-        <v>55</v>
+      <c r="C56" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" t="s">
+        <v>32</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D57" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" t="s">
+        <v>57</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D58" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1239,6 +1460,19 @@
     <hyperlink ref="C43" r:id="rId42"/>
     <hyperlink ref="C44" r:id="rId43"/>
     <hyperlink ref="C45" r:id="rId44"/>
+    <hyperlink ref="C46" r:id="rId45"/>
+    <hyperlink ref="C47" r:id="rId46"/>
+    <hyperlink ref="C48" r:id="rId47"/>
+    <hyperlink ref="C49" r:id="rId48"/>
+    <hyperlink ref="C50" r:id="rId49"/>
+    <hyperlink ref="C51" r:id="rId50"/>
+    <hyperlink ref="C52" r:id="rId51"/>
+    <hyperlink ref="C53" r:id="rId52"/>
+    <hyperlink ref="C54" r:id="rId53"/>
+    <hyperlink ref="C55" r:id="rId54"/>
+    <hyperlink ref="C56" r:id="rId55"/>
+    <hyperlink ref="C57" r:id="rId56"/>
+    <hyperlink ref="C58" r:id="rId57"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>